<commit_message>
Added State Fund Profile
</commit_message>
<xml_diff>
--- a/src/main/java/TestSuite/RegressionScenarios.xlsx
+++ b/src/main/java/TestSuite/RegressionScenarios.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\athakur\Documents\MDOT\rstar\rstars\src\main\java\TestSuite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pdighe\Documents\MDOT\Rstars-Automation\src\main\java\TestSuite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CDAF03F-F471-468E-ABD8-2B7D42829962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E693C532-59FE-4BFA-B5A3-20FB23952C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="18780" windowHeight="9920" xr2:uid="{25BA6363-D021-4585-A3A2-80239D66B0B0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{25BA6363-D021-4585-A3A2-80239D66B0B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="59">
   <si>
     <t>Scenario Type</t>
   </si>
@@ -190,13 +190,34 @@
   </si>
   <si>
     <t>GAAP GL Account Class Profile</t>
+  </si>
+  <si>
+    <t>Project Type Profile</t>
+  </si>
+  <si>
+    <t>Object Profile</t>
+  </si>
+  <si>
+    <t>GAAP Category Profile</t>
+  </si>
+  <si>
+    <t>TS_SM_FOU_AppropriationGroupProfile_Regression_001</t>
+  </si>
+  <si>
+    <t>Appropriation Group Profile</t>
+  </si>
+  <si>
+    <t>TS_SM_FOU_StateFundGroupProfile_Regression_001</t>
+  </si>
+  <si>
+    <t>State Fund Group Profile</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,6 +245,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -246,8 +274,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -289,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -297,10 +325,11 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26B130D1-9A15-4CB4-A42C-CA3AEBC8C272}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -643,199 +672,199 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="D3" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="C8" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="A10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="4" t="s">
+      <c r="A11" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="3" t="s">
+      <c r="C13" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -844,10 +873,10 @@
         <v>4</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>7</v>
@@ -858,10 +887,10 @@
         <v>4</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>7</v>
@@ -872,10 +901,10 @@
         <v>4</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>7</v>
@@ -886,10 +915,10 @@
         <v>4</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>7</v>
@@ -900,10 +929,10 @@
         <v>4</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>7</v>
@@ -914,10 +943,10 @@
         <v>4</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>7</v>
@@ -928,58 +957,86 @@
         <v>4</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="3" t="s">
+      <c r="D24" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="6" t="s">
+      <c r="D25" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="6" t="s">
+      <c r="D26" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Grant Control Profile 90% done
</commit_message>
<xml_diff>
--- a/src/main/java/TestSuite/RegressionScenarios.xlsx
+++ b/src/main/java/TestSuite/RegressionScenarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdeepika\Documents\Rstars-Automation\src\main\java\TestSuite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pdighe\Documents\MDOT\Rstars-Automation\src\main\java\TestSuite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8099C5E7-17EE-49D8-A495-2475059C1590}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7F1C5B-50C1-46C6-9507-2B5E12459B1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12" yWindow="12" windowWidth="23016" windowHeight="12336" xr2:uid="{25BA6363-D021-4585-A3A2-80239D66B0B0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{25BA6363-D021-4585-A3A2-80239D66B0B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="65">
   <si>
     <t>Scenario Type</t>
   </si>
@@ -223,6 +223,12 @@
   </si>
   <si>
     <t>Contract Profile</t>
+  </si>
+  <si>
+    <t>TS_PM_COA_PRI_GrantControlProfile_Regression_001</t>
+  </si>
+  <si>
+    <t>Grant Control Profile</t>
   </si>
 </sst>
 </file>
@@ -351,7 +357,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -666,21 +672,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26B130D1-9A15-4CB4-A42C-CA3AEBC8C272}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="69.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -694,7 +700,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -708,7 +714,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -722,7 +728,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
@@ -736,7 +742,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
@@ -750,7 +756,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
@@ -764,7 +770,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>4</v>
       </c>
@@ -778,7 +784,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>4</v>
       </c>
@@ -792,297 +798,311 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="7" t="s">
+      <c r="D10" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="7" t="s">
+      <c r="D11" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C12" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="7" t="s">
+      <c r="D12" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C13" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="7" t="s">
+      <c r="D13" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C14" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="4" t="s">
+      <c r="D14" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="4" t="s">
+      <c r="D15" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="3" t="s">
+      <c r="D16" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="3" t="s">
+      <c r="D17" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="3" t="s">
+      <c r="D18" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="3" t="s">
+      <c r="D19" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="3" t="s">
+      <c r="D20" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="3" t="s">
+      <c r="D21" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="3" t="s">
+      <c r="D22" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="3" t="s">
+      <c r="D23" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="3" t="s">
+      <c r="D24" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="3" t="s">
+      <c r="D25" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" s="5" t="s">
+      <c r="D26" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="5" t="s">
+      <c r="D27" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="5" t="s">
+      <c r="D28" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D29" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C30" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D30" s="8" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>